<commit_message>
fixed lg names for Dompo and Tsikimba
</commit_message>
<xml_diff>
--- a/raw/xlsx/numerals-domp1238-1.xlsx
+++ b/raw/xlsx/numerals-domp1238-1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bibiko/Downloads/Upload-Excel-Sept-14-2021/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bibiko/Documents/Developments/shh_git/numeralbank/numerals/raw/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAE49921-0B3C-B740-BA95-DD557BE78FC3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0863DC07-E3C2-FA43-9FFD-0D9A29A88462}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-8020" yWindow="-22480" windowWidth="31020" windowHeight="17160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-8020" yWindow="-22480" windowWidth="31020" windowHeight="17160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -92,9 +92,6 @@
     <t>doy</t>
   </si>
   <si>
-    <t>Dompo</t>
-  </si>
-  <si>
     <t>敦波语</t>
   </si>
   <si>
@@ -282,6 +279,9 @@
   </si>
   <si>
     <t>youngest consultant</t>
+  </si>
+  <si>
+    <t>Dompo, Bono Region, Ghana</t>
   </si>
 </sst>
 </file>
@@ -708,7 +708,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
     </sheetView>
@@ -745,7 +745,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="3"/>
@@ -756,7 +756,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -767,7 +767,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -778,10 +778,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
@@ -791,10 +791,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -804,10 +804,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
@@ -817,10 +817,10 @@
         <v>5</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
@@ -830,7 +830,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="3"/>
@@ -841,7 +841,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="3"/>
@@ -852,7 +852,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -863,7 +863,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -874,7 +874,7 @@
         <v>10</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -885,7 +885,7 @@
         <v>11</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
@@ -896,7 +896,7 @@
         <v>12</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -907,7 +907,7 @@
         <v>12</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C16" s="8"/>
       <c r="D16" s="3"/>
@@ -918,7 +918,7 @@
         <v>14</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C17" s="8"/>
       <c r="D17" s="7"/>
@@ -929,7 +929,7 @@
         <v>14</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C18" s="8"/>
       <c r="D18" s="3"/>
@@ -939,7 +939,7 @@
         <v>15</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C19" s="8"/>
       <c r="D19" s="7"/>
@@ -949,7 +949,7 @@
         <v>15</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C20" s="8"/>
     </row>
@@ -958,7 +958,7 @@
         <v>16</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C21" s="7" t="s">
         <v>20</v>
@@ -969,7 +969,7 @@
         <v>17</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
@@ -977,7 +977,7 @@
         <v>18</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
@@ -985,7 +985,7 @@
         <v>19</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
@@ -993,7 +993,7 @@
         <v>20</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
@@ -1003,7 +1003,7 @@
         <v>21</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
@@ -1011,7 +1011,7 @@
         <v>22</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
@@ -1019,7 +1019,7 @@
         <v>23</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
@@ -1027,7 +1027,7 @@
         <v>24</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
@@ -1035,7 +1035,7 @@
         <v>25</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
@@ -1043,7 +1043,7 @@
         <v>26</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
@@ -1051,7 +1051,7 @@
         <v>27</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="30" x14ac:dyDescent="0.55000000000000004">
@@ -1059,7 +1059,7 @@
         <v>28</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.55000000000000004">
@@ -1067,7 +1067,7 @@
         <v>29</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.55000000000000004">
@@ -1075,7 +1075,7 @@
         <v>30</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.55000000000000004">
@@ -1083,7 +1083,7 @@
         <v>31</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.55000000000000004">
@@ -1091,10 +1091,10 @@
         <v>40</v>
       </c>
       <c r="B37" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="C37" s="16" t="s">
         <v>73</v>
-      </c>
-      <c r="C37" s="16" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.55000000000000004">
@@ -1102,7 +1102,7 @@
         <v>50</v>
       </c>
       <c r="B38" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C38" s="7" t="s">
         <v>20</v>
@@ -1116,10 +1116,10 @@
         <v>60</v>
       </c>
       <c r="B39" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C39" s="16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D39" s="7"/>
     </row>
@@ -1128,7 +1128,7 @@
         <v>70</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D40" s="7"/>
     </row>
@@ -1137,10 +1137,10 @@
         <v>80</v>
       </c>
       <c r="B41" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C41" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D41" s="7"/>
     </row>
@@ -1149,7 +1149,7 @@
         <v>90</v>
       </c>
       <c r="B42" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C42" s="7" t="s">
         <v>20</v>
@@ -1160,7 +1160,7 @@
         <v>100</v>
       </c>
       <c r="B43" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D43" s="7">
         <v>1</v>
@@ -1171,7 +1171,7 @@
         <v>101</v>
       </c>
       <c r="B44" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="30" x14ac:dyDescent="0.55000000000000004">
@@ -1179,7 +1179,7 @@
         <v>200</v>
       </c>
       <c r="B45" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C45" s="9"/>
     </row>
@@ -1188,7 +1188,7 @@
         <v>400</v>
       </c>
       <c r="B46" s="13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C46" s="9"/>
     </row>
@@ -1197,7 +1197,7 @@
         <v>1000</v>
       </c>
       <c r="B47" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C47" s="9"/>
       <c r="D47" s="7"/>
@@ -1207,7 +1207,7 @@
         <v>2000</v>
       </c>
       <c r="B48" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C48" s="9"/>
     </row>
@@ -1216,7 +1216,7 @@
         <v>7013</v>
       </c>
       <c r="B49" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C49" s="9"/>
     </row>
@@ -1252,8 +1252,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1283,7 +1283,7 @@
         <v>7</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>23</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="31" x14ac:dyDescent="0.2">
@@ -1291,7 +1291,7 @@
         <v>8</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="31" x14ac:dyDescent="0.2">
@@ -1299,7 +1299,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="31" x14ac:dyDescent="0.2">
@@ -1307,7 +1307,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.55000000000000004">
@@ -1315,7 +1315,7 @@
         <v>11</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.55000000000000004">
@@ -1323,7 +1323,7 @@
         <v>12</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="30" x14ac:dyDescent="0.55000000000000004">
@@ -1331,7 +1331,7 @@
         <v>13</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.2">
@@ -1351,7 +1351,7 @@
         <v>16</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="31" x14ac:dyDescent="0.2">
@@ -1359,7 +1359,7 @@
         <v>17</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="31" x14ac:dyDescent="0.2">
@@ -1367,7 +1367,7 @@
         <v>18</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1375,7 +1375,7 @@
         <v>19</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>